<commit_message>
Update DDL script and Arena of Valor project files
Expanded the DDL teaching script with detailed SQLite DDL operations, including CREATE, ALTER, TRUNCATE, COMMENT, RENAME, and DROP examples. Updated related slides and dataset files for Arena of Valor, modified the project database, and removed the obsolete database journal file.
</commit_message>
<xml_diff>
--- a/Project/Arena of Valor/Dataset_ArenaofValor.xlsx
+++ b/Project/Arena of Valor/Dataset_ArenaofValor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaotingzhou/Documents/Lectures/SQL/Project/Arena of Valor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6BD67D-93D9-184E-AF00-28CD8B5ADCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26668BC7-6580-9349-9EE6-7FAFEA4ACE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" activeTab="1" xr2:uid="{4F4E6C32-125B-FC44-9721-F24B365705FA}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="259">
   <si>
     <t>字段名</t>
   </si>
@@ -992,12 +992,33 @@
       <t>,</t>
     </r>
   </si>
+  <si>
+    <t>1 match</t>
+  </si>
+  <si>
+    <t>10 players</t>
+  </si>
+  <si>
+    <t>1 player</t>
+  </si>
+  <si>
+    <t>1 hero</t>
+  </si>
+  <si>
+    <t>6 items</t>
+  </si>
+  <si>
+    <t>2 master_skill</t>
+  </si>
+  <si>
+    <t>5 vs 5 (red vs blue)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="28">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1159,8 +1180,21 @@
       <color rgb="FFC00000"/>
       <name val="Aptos Narrow (Body)"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="26"/>
+      <color theme="4"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1176,6 +1210,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1207,7 +1247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1241,6 +1281,15 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2277,22 +2326,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E5690EB-2240-5344-BE84-8D3D170BFF8E}">
   <dimension ref="A1:Z133"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="56" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="34"/>
   <cols>
     <col min="1" max="12" width="10.83203125" style="3"/>
     <col min="13" max="13" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="34.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.1640625" style="3" customWidth="1"/>
     <col min="16" max="16" width="19" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.1640625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="42.33203125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="31" style="3" customWidth="1"/>
+    <col min="20" max="20" width="29.83203125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="25.5" style="3" customWidth="1"/>
+    <col min="22" max="22" width="38" style="3" customWidth="1"/>
+    <col min="23" max="23" width="35.6640625" style="3" customWidth="1"/>
     <col min="24" max="24" width="30.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="27.5" style="3" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="33.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -2539,7 +2590,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:22">
       <c r="B17" s="3" t="s">
         <v>44</v>
       </c>
@@ -2550,7 +2601,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:22">
       <c r="B18" s="3" t="s">
         <v>45</v>
       </c>
@@ -2561,7 +2612,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:22">
       <c r="B19" s="3" t="s">
         <v>46</v>
       </c>
@@ -2572,7 +2623,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:22">
       <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
@@ -2583,7 +2634,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:22">
       <c r="A21" s="11"/>
       <c r="B21" s="3" t="s">
         <v>47</v>
@@ -2595,7 +2646,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:22">
       <c r="B22" s="3" t="s">
         <v>48</v>
       </c>
@@ -2606,7 +2657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:22">
       <c r="B23" s="3" t="s">
         <v>2</v>
       </c>
@@ -2617,7 +2668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:22">
       <c r="B24" s="3" t="s">
         <v>49</v>
       </c>
@@ -2628,37 +2679,65 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:22">
       <c r="B25" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:22">
       <c r="B26" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:22">
       <c r="B27" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:22">
       <c r="B28" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="29" spans="1:14">
+      <c r="R28" s="32"/>
+      <c r="S28" s="32"/>
+      <c r="T28" s="32"/>
+    </row>
+    <row r="29" spans="1:22">
       <c r="B29" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="R29" s="32"/>
+      <c r="S29" s="32"/>
+      <c r="T29" s="32"/>
+    </row>
+    <row r="30" spans="1:22">
       <c r="B30" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="Q30" s="32"/>
+      <c r="R30" s="32"/>
+      <c r="S30" s="32"/>
+      <c r="T30" s="32"/>
+      <c r="U30" s="32"/>
+      <c r="V30" s="32"/>
+    </row>
+    <row r="31" spans="1:22">
+      <c r="Q31" s="33"/>
+      <c r="R31" s="32"/>
+      <c r="S31" s="32"/>
+      <c r="T31" s="32"/>
+      <c r="U31" s="32"/>
+      <c r="V31" s="32"/>
+    </row>
+    <row r="32" spans="1:22">
+      <c r="Q32" s="32"/>
+      <c r="R32" s="32"/>
+      <c r="S32" s="32"/>
+      <c r="T32" s="32"/>
+      <c r="U32" s="32"/>
+      <c r="V32" s="32"/>
+    </row>
+    <row r="33" spans="1:22">
       <c r="M33" s="14" t="s">
         <v>6</v>
       </c>
@@ -2668,8 +2747,14 @@
       <c r="O33" s="14" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="Q33" s="32"/>
+      <c r="R33" s="32"/>
+      <c r="S33" s="32"/>
+      <c r="T33" s="32"/>
+      <c r="U33" s="32"/>
+      <c r="V33" s="32"/>
+    </row>
+    <row r="34" spans="1:22">
       <c r="B34" s="3" t="s">
         <v>22</v>
       </c>
@@ -2682,8 +2767,14 @@
       <c r="O34" s="12" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="35" spans="1:15">
+      <c r="Q34" s="32"/>
+      <c r="R34" s="32"/>
+      <c r="S34" s="32"/>
+      <c r="T34" s="32"/>
+      <c r="U34" s="32"/>
+      <c r="V34" s="32"/>
+    </row>
+    <row r="35" spans="1:22">
       <c r="A35" s="10"/>
       <c r="B35" s="3" t="s">
         <v>52</v>
@@ -2697,8 +2788,14 @@
       <c r="O35" s="12" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="Q35" s="32"/>
+      <c r="R35" s="32"/>
+      <c r="S35" s="32"/>
+      <c r="T35" s="32"/>
+      <c r="U35" s="32"/>
+      <c r="V35" s="32"/>
+    </row>
+    <row r="36" spans="1:22">
       <c r="A36" s="10"/>
       <c r="B36" s="3" t="s">
         <v>53</v>
@@ -2712,8 +2809,14 @@
       <c r="O36" s="12" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="Q36" s="32"/>
+      <c r="R36" s="32"/>
+      <c r="S36" s="32"/>
+      <c r="T36" s="32"/>
+      <c r="U36" s="32"/>
+      <c r="V36" s="32"/>
+    </row>
+    <row r="37" spans="1:22">
       <c r="A37" s="10"/>
       <c r="B37" s="3" t="s">
         <v>54</v>
@@ -2727,8 +2830,14 @@
       <c r="O37" s="12" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="38" spans="1:15">
+      <c r="Q37" s="32"/>
+      <c r="R37" s="32"/>
+      <c r="S37" s="32"/>
+      <c r="T37" s="32"/>
+      <c r="U37" s="32"/>
+      <c r="V37" s="32"/>
+    </row>
+    <row r="38" spans="1:22">
       <c r="B38" s="3" t="s">
         <v>21</v>
       </c>
@@ -2741,8 +2850,14 @@
       <c r="O38" s="12" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="39" spans="1:15">
+      <c r="Q38" s="32"/>
+      <c r="R38" s="32"/>
+      <c r="S38" s="32"/>
+      <c r="T38" s="32"/>
+      <c r="U38" s="32"/>
+      <c r="V38" s="32"/>
+    </row>
+    <row r="39" spans="1:22">
       <c r="M39" s="12">
         <v>6</v>
       </c>
@@ -2752,8 +2867,14 @@
       <c r="O39" s="12" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="40" spans="1:15">
+      <c r="Q39" s="32"/>
+      <c r="R39" s="32"/>
+      <c r="S39" s="32"/>
+      <c r="T39" s="32"/>
+      <c r="U39" s="32"/>
+      <c r="V39" s="32"/>
+    </row>
+    <row r="40" spans="1:22">
       <c r="M40" s="12">
         <v>7</v>
       </c>
@@ -2763,8 +2884,14 @@
       <c r="O40" s="12" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="41" spans="1:15">
+      <c r="Q40" s="32"/>
+      <c r="R40" s="32"/>
+      <c r="S40" s="32"/>
+      <c r="T40" s="32"/>
+      <c r="U40" s="32"/>
+      <c r="V40" s="32"/>
+    </row>
+    <row r="41" spans="1:22">
       <c r="M41" s="12">
         <v>8</v>
       </c>
@@ -2774,8 +2901,14 @@
       <c r="O41" s="12" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="42" spans="1:15">
+      <c r="Q41" s="32"/>
+      <c r="R41" s="32"/>
+      <c r="S41" s="32"/>
+      <c r="T41" s="32"/>
+      <c r="U41" s="32"/>
+      <c r="V41" s="32"/>
+    </row>
+    <row r="42" spans="1:22">
       <c r="M42" s="12">
         <v>9</v>
       </c>
@@ -2785,19 +2918,47 @@
       <c r="O42" s="12" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="45" spans="1:15">
+      <c r="Q42" s="32"/>
+      <c r="R42" s="32"/>
+      <c r="S42" s="32"/>
+      <c r="T42" s="32"/>
+      <c r="U42" s="32"/>
+      <c r="V42" s="32"/>
+    </row>
+    <row r="43" spans="1:22">
+      <c r="Q43" s="32"/>
+      <c r="R43" s="32"/>
+      <c r="S43" s="32"/>
+      <c r="T43" s="32"/>
+      <c r="U43" s="32"/>
+      <c r="V43" s="32"/>
+    </row>
+    <row r="44" spans="1:22">
+      <c r="Q44" s="32"/>
+      <c r="R44" s="32"/>
+      <c r="S44" s="32"/>
+      <c r="T44" s="32"/>
+      <c r="U44" s="32"/>
+      <c r="V44" s="32"/>
+    </row>
+    <row r="45" spans="1:22">
       <c r="M45" s="14" t="s">
         <v>15</v>
       </c>
       <c r="N45" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="O45" s="14" t="s">
+      <c r="O45" s="31" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="46" spans="1:15">
+      <c r="Q45" s="33"/>
+      <c r="R45" s="33"/>
+      <c r="S45" s="32"/>
+      <c r="T45" s="32"/>
+      <c r="U45" s="32"/>
+      <c r="V45" s="32"/>
+    </row>
+    <row r="46" spans="1:22">
       <c r="B46" s="3" t="s">
         <v>70</v>
       </c>
@@ -2810,8 +2971,14 @@
       <c r="O46" s="12" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="47" spans="1:15">
+      <c r="Q46" s="32"/>
+      <c r="R46" s="32"/>
+      <c r="S46" s="32"/>
+      <c r="T46" s="32"/>
+      <c r="U46" s="32"/>
+      <c r="V46" s="32"/>
+    </row>
+    <row r="47" spans="1:22">
       <c r="B47" s="3" t="s">
         <v>71</v>
       </c>
@@ -2824,8 +2991,14 @@
       <c r="O47" s="12" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="48" spans="1:15">
+      <c r="Q47" s="32"/>
+      <c r="R47" s="32"/>
+      <c r="S47" s="32"/>
+      <c r="T47" s="32"/>
+      <c r="U47" s="32"/>
+      <c r="V47" s="32"/>
+    </row>
+    <row r="48" spans="1:22">
       <c r="B48" s="3" t="s">
         <v>72</v>
       </c>
@@ -2838,8 +3011,14 @@
       <c r="O48" s="12" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="49" spans="1:15">
+      <c r="Q48" s="32"/>
+      <c r="R48" s="32"/>
+      <c r="S48" s="32"/>
+      <c r="T48" s="32"/>
+      <c r="U48" s="32"/>
+      <c r="V48" s="32"/>
+    </row>
+    <row r="49" spans="1:22">
       <c r="B49" s="3" t="s">
         <v>73</v>
       </c>
@@ -2852,8 +3031,14 @@
       <c r="O49" s="12" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="50" spans="1:15">
+      <c r="Q49" s="32"/>
+      <c r="R49" s="32"/>
+      <c r="S49" s="32"/>
+      <c r="T49" s="32"/>
+      <c r="U49" s="32"/>
+      <c r="V49" s="32"/>
+    </row>
+    <row r="50" spans="1:22">
       <c r="B50" s="3" t="s">
         <v>21</v>
       </c>
@@ -2866,8 +3051,14 @@
       <c r="O50" s="12" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="51" spans="1:15">
+      <c r="Q50" s="32"/>
+      <c r="R50" s="32"/>
+      <c r="S50" s="32"/>
+      <c r="T50" s="32"/>
+      <c r="U50" s="32"/>
+      <c r="V50" s="32"/>
+    </row>
+    <row r="51" spans="1:22">
       <c r="M51" s="12">
         <v>6</v>
       </c>
@@ -2877,8 +3068,14 @@
       <c r="O51" s="12" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="52" spans="1:15">
+      <c r="Q51" s="32"/>
+      <c r="R51" s="32"/>
+      <c r="S51" s="32"/>
+      <c r="T51" s="32"/>
+      <c r="U51" s="32"/>
+      <c r="V51" s="32"/>
+    </row>
+    <row r="52" spans="1:22">
       <c r="M52" s="12">
         <v>7</v>
       </c>
@@ -2888,8 +3085,14 @@
       <c r="O52" s="12" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="53" spans="1:15">
+      <c r="Q52" s="32"/>
+      <c r="R52" s="32"/>
+      <c r="S52" s="32"/>
+      <c r="T52" s="32"/>
+      <c r="U52" s="32"/>
+      <c r="V52" s="32"/>
+    </row>
+    <row r="53" spans="1:22">
       <c r="M53" s="12">
         <v>8</v>
       </c>
@@ -2899,8 +3102,14 @@
       <c r="O53" s="12" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="54" spans="1:15">
+      <c r="Q53" s="32"/>
+      <c r="R53" s="32"/>
+      <c r="S53" s="32"/>
+      <c r="T53" s="32"/>
+      <c r="U53" s="32"/>
+      <c r="V53" s="32"/>
+    </row>
+    <row r="54" spans="1:22">
       <c r="M54" s="12">
         <v>9</v>
       </c>
@@ -2910,8 +3119,14 @@
       <c r="O54" s="12" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="55" spans="1:15">
+      <c r="Q54" s="32"/>
+      <c r="R54" s="32"/>
+      <c r="S54" s="32"/>
+      <c r="T54" s="32"/>
+      <c r="U54" s="32"/>
+      <c r="V54" s="32"/>
+    </row>
+    <row r="55" spans="1:22">
       <c r="M55" s="12">
         <v>10</v>
       </c>
@@ -2921,11 +3136,31 @@
       <c r="O55" s="12" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="57" spans="1:15">
+      <c r="Q55" s="32"/>
+      <c r="R55" s="32"/>
+      <c r="S55" s="32"/>
+      <c r="T55" s="32"/>
+      <c r="U55" s="32"/>
+      <c r="V55" s="32"/>
+    </row>
+    <row r="56" spans="1:22">
+      <c r="Q56" s="32"/>
+      <c r="R56" s="32"/>
+      <c r="S56" s="32"/>
+      <c r="T56" s="32"/>
+      <c r="U56" s="32"/>
+      <c r="V56" s="32"/>
+    </row>
+    <row r="57" spans="1:22">
       <c r="A57" s="4"/>
-    </row>
-    <row r="58" spans="1:15">
+      <c r="Q57" s="32"/>
+      <c r="R57" s="32"/>
+      <c r="S57" s="32"/>
+      <c r="T57" s="32"/>
+      <c r="U57" s="32"/>
+      <c r="V57" s="32"/>
+    </row>
+    <row r="58" spans="1:22">
       <c r="A58" s="4"/>
       <c r="M58" s="14" t="s">
         <v>102</v>
@@ -2936,8 +3171,14 @@
       <c r="O58" s="14" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="59" spans="1:15">
+      <c r="Q58" s="32"/>
+      <c r="R58" s="32"/>
+      <c r="S58" s="32"/>
+      <c r="T58" s="32"/>
+      <c r="U58" s="32"/>
+      <c r="V58" s="32"/>
+    </row>
+    <row r="59" spans="1:22">
       <c r="A59" s="4"/>
       <c r="M59" s="12">
         <v>1</v>
@@ -2949,7 +3190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:22">
       <c r="A60" s="4"/>
       <c r="B60" s="3" t="s">
         <v>89</v>
@@ -2964,7 +3205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:22">
       <c r="A61" s="4"/>
       <c r="B61" s="3" t="s">
         <v>90</v>
@@ -2979,7 +3220,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:22">
       <c r="A62" s="4"/>
       <c r="B62" s="3" t="s">
         <v>91</v>
@@ -2994,7 +3235,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:22">
       <c r="B63" s="3" t="s">
         <v>92</v>
       </c>
@@ -3008,7 +3249,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:22">
       <c r="B64" s="3" t="s">
         <v>93</v>
       </c>
@@ -3578,90 +3819,200 @@
         <v>113</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:20">
       <c r="B81" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="82" spans="1:2">
+      <c r="M81" s="34"/>
+      <c r="N81" s="34"/>
+      <c r="O81" s="34"/>
+      <c r="P81" s="34"/>
+      <c r="Q81" s="34"/>
+      <c r="R81" s="34"/>
+      <c r="S81" s="34"/>
+      <c r="T81" s="34"/>
+    </row>
+    <row r="82" spans="1:20">
       <c r="A82" s="5"/>
       <c r="B82" s="3" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
+      <c r="M82" s="34"/>
+      <c r="N82" s="34"/>
+      <c r="O82" s="34"/>
+      <c r="P82" s="34"/>
+      <c r="Q82" s="34"/>
+      <c r="R82" s="34"/>
+      <c r="S82" s="34"/>
+      <c r="T82" s="34"/>
+    </row>
+    <row r="83" spans="1:20">
       <c r="B83" s="3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="84" spans="1:2">
+      <c r="M83" s="34"/>
+      <c r="N83" s="34"/>
+      <c r="O83" s="34"/>
+      <c r="P83" s="34"/>
+      <c r="Q83" s="34"/>
+      <c r="R83" s="34"/>
+      <c r="S83" s="34"/>
+      <c r="T83" s="34"/>
+    </row>
+    <row r="84" spans="1:20">
       <c r="A84" s="5"/>
       <c r="B84" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="85" spans="1:2">
+      <c r="M84" s="34"/>
+      <c r="N84" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="O84" s="35" t="s">
+        <v>253</v>
+      </c>
+      <c r="P84" s="35" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q84" s="35"/>
+      <c r="R84" s="35"/>
+      <c r="S84" s="34"/>
+      <c r="T84" s="34"/>
+    </row>
+    <row r="85" spans="1:20">
       <c r="B85" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="86" spans="1:2">
+      <c r="M85" s="34"/>
+      <c r="N85" s="35"/>
+      <c r="O85" s="35"/>
+      <c r="P85" s="35"/>
+      <c r="Q85" s="35"/>
+      <c r="R85" s="35"/>
+      <c r="S85" s="34"/>
+      <c r="T85" s="34"/>
+    </row>
+    <row r="86" spans="1:20">
       <c r="A86" s="5"/>
       <c r="B86" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="87" spans="1:2">
+      <c r="M86" s="34"/>
+      <c r="N86" s="35"/>
+      <c r="O86" s="35" t="s">
+        <v>254</v>
+      </c>
+      <c r="P86" s="35" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q86" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="R86" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="S86" s="34"/>
+      <c r="T86" s="34"/>
+    </row>
+    <row r="87" spans="1:20">
       <c r="B87" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" ht="38">
+      <c r="M87" s="34"/>
+      <c r="N87" s="34"/>
+      <c r="O87" s="34"/>
+      <c r="P87" s="34"/>
+      <c r="Q87" s="34"/>
+      <c r="R87" s="34"/>
+      <c r="S87" s="34"/>
+      <c r="T87" s="34"/>
+    </row>
+    <row r="88" spans="1:20" ht="38">
       <c r="A88" s="6"/>
       <c r="B88" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" ht="38">
+      <c r="M88" s="34"/>
+      <c r="N88" s="34"/>
+      <c r="O88" s="34"/>
+      <c r="P88" s="34"/>
+      <c r="Q88" s="34"/>
+      <c r="R88" s="34"/>
+      <c r="S88" s="34"/>
+      <c r="T88" s="34"/>
+    </row>
+    <row r="89" spans="1:20" ht="38">
       <c r="A89" s="6"/>
       <c r="B89" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" ht="38">
+      <c r="M89" s="34"/>
+      <c r="N89" s="34"/>
+      <c r="O89" s="34"/>
+      <c r="P89" s="34"/>
+      <c r="Q89" s="34"/>
+      <c r="R89" s="34"/>
+      <c r="S89" s="34"/>
+      <c r="T89" s="34"/>
+    </row>
+    <row r="90" spans="1:20" ht="38">
       <c r="A90" s="6"/>
       <c r="B90" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" ht="38">
+      <c r="M90" s="34"/>
+      <c r="N90" s="34"/>
+      <c r="O90" s="34"/>
+      <c r="P90" s="34"/>
+      <c r="Q90" s="34"/>
+      <c r="R90" s="34"/>
+      <c r="S90" s="34"/>
+      <c r="T90" s="34"/>
+    </row>
+    <row r="91" spans="1:20" ht="38">
       <c r="A91" s="6"/>
       <c r="B91" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" ht="38">
+      <c r="M91" s="34"/>
+      <c r="N91" s="34"/>
+      <c r="O91" s="34"/>
+      <c r="P91" s="34"/>
+      <c r="Q91" s="34"/>
+      <c r="R91" s="34"/>
+      <c r="S91" s="34"/>
+      <c r="T91" s="34"/>
+    </row>
+    <row r="92" spans="1:20" ht="38">
       <c r="A92" s="6"/>
       <c r="B92" s="3" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="93" spans="1:2">
+      <c r="M92" s="34"/>
+      <c r="N92" s="34"/>
+      <c r="O92" s="34"/>
+      <c r="P92" s="34"/>
+      <c r="Q92" s="34"/>
+      <c r="R92" s="34"/>
+      <c r="S92" s="34"/>
+      <c r="T92" s="34"/>
+    </row>
+    <row r="93" spans="1:20">
       <c r="B93" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:20">
       <c r="B94" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:20">
       <c r="B95" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:20">
       <c r="A96" s="5"/>
       <c r="B96" s="3" t="s">
         <v>119</v>
@@ -3739,6 +4090,7 @@
       <c r="A133" s="6"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>